<commit_message>
Revert "Merge branch 'main' into feature/fix-note-optionals"
This reverts commit f1bdb8af30d322360f452311725b3a0028fabc80, reversing
changes made to e6451804c522a90724bf106b62579b03d91b317c.
</commit_message>
<xml_diff>
--- a/CodeDocumentation/2024 Cresendo.xlsx
+++ b/CodeDocumentation/2024 Cresendo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="164">
   <si>
     <t>Note Managment</t>
   </si>
@@ -266,9 +266,6 @@
     <t>Practice Bot</t>
   </si>
   <si>
-    <t>Comp Bot</t>
-  </si>
-  <si>
     <t>Distance (m)</t>
   </si>
   <si>
@@ -276,6 +273,12 @@
   </si>
   <si>
     <t>distance</t>
+  </si>
+  <si>
+    <t>5:1</t>
+  </si>
+  <si>
+    <t>1:1</t>
   </si>
   <si>
     <t>angle</t>
@@ -770,11 +773,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1117060003"/>
-        <c:axId val="310689654"/>
+        <c:axId val="1810185014"/>
+        <c:axId val="541479536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1117060003"/>
+        <c:axId val="1810185014"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,10 +852,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310689654"/>
+        <c:crossAx val="541479536"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="310689654"/>
+        <c:axId val="541479536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -927,7 +930,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1117060003"/>
+        <c:crossAx val="1810185014"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -12411,55 +12414,32 @@
       <c r="A1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="11" t="s">
+    </row>
+    <row r="4">
+      <c r="M4" s="12" t="s">
         <v>85</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="D3" s="12">
-        <v>3.25</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="D4" s="12">
-        <v>2.45</v>
-      </c>
-      <c r="E4" s="12">
-        <v>10.0</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="N4" s="12">
         <v>1.88</v>
       </c>
     </row>
     <row r="5">
-      <c r="D5" s="12">
-        <v>1.74</v>
-      </c>
-      <c r="E5" s="12">
-        <v>19.0</v>
+      <c r="E5" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N5" s="13">
         <f>N4*(-15.8)-3.14</f>
@@ -12467,17 +12447,295 @@
       </c>
     </row>
     <row r="6">
+      <c r="A6" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="B6" s="12">
+        <v>-20.0</v>
+      </c>
       <c r="D6" s="12">
-        <v>1.26</v>
+        <v>1.3</v>
       </c>
       <c r="E6" s="12">
-        <v>35.0</v>
+        <v>-26.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="E7" s="12">
+        <v>-20.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="E8" s="12">
+        <v>-25.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="12">
+        <v>1.55</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1.6</v>
+      </c>
+      <c r="E9" s="12">
+        <v>-31.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="12">
+        <v>1.6</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1.7</v>
+      </c>
+      <c r="E10" s="12">
+        <v>-31.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="12">
+        <v>1.65</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="E11" s="12">
+        <v>-31.75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="12">
+        <v>1.745</v>
+      </c>
+      <c r="B12" s="12">
+        <v>-30.0</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="E12" s="12">
+        <v>-32.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="13">
+        <f t="shared" ref="A13:A27" si="1">A12+12*0.0254</f>
+        <v>2.0498</v>
+      </c>
+      <c r="B13" s="12">
+        <v>-40.0</v>
+      </c>
+      <c r="D13" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E13" s="12">
+        <v>-35.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="13">
+        <f t="shared" si="1"/>
+        <v>2.3546</v>
+      </c>
+      <c r="B14" s="12">
+        <v>39.5</v>
+      </c>
+      <c r="D14" s="12">
+        <v>2.1</v>
+      </c>
+      <c r="E14" s="12">
+        <v>-39.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="13">
+        <f t="shared" si="1"/>
+        <v>2.6594</v>
+      </c>
+      <c r="D15" s="12">
+        <v>2.2</v>
+      </c>
+      <c r="E15" s="12">
+        <v>-40.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="13">
+        <f t="shared" si="1"/>
+        <v>2.9642</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2.54</v>
+      </c>
+      <c r="E16" s="12">
+        <v>-44.5</v>
+      </c>
+      <c r="F16" s="12">
+        <v>-44.5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="13">
+        <f t="shared" si="1"/>
+        <v>3.269</v>
+      </c>
+      <c r="D17" s="12">
+        <v>3.2</v>
+      </c>
+      <c r="E17" s="12">
+        <v>-50.5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="13">
+        <f t="shared" si="1"/>
+        <v>3.5738</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="13">
+        <f t="shared" si="1"/>
+        <v>3.8786</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="13">
+        <f t="shared" si="1"/>
+        <v>4.1834</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="13">
+        <f t="shared" si="1"/>
+        <v>4.4882</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" ref="E21:E22" si="2">D9</f>
+        <v>1.6</v>
+      </c>
+      <c r="F21" s="13">
+        <f t="shared" ref="F21:F29" si="3">6.72-27.1*D9+2.85*D9*D9</f>
+        <v>-29.344</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="13">
+        <f t="shared" si="1"/>
+        <v>4.793</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="2"/>
+        <v>1.7</v>
+      </c>
+      <c r="F22" s="13">
+        <f t="shared" si="3"/>
+        <v>-31.1135</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="13">
+        <f t="shared" si="1"/>
+        <v>5.0978</v>
+      </c>
+      <c r="E23" s="12">
+        <v>1.88</v>
+      </c>
+      <c r="F23" s="13">
+        <f t="shared" si="3"/>
+        <v>-32.826</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="13">
+        <f t="shared" si="1"/>
+        <v>5.4026</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" ref="E24:E30" si="4">D12</f>
+        <v>1.9</v>
+      </c>
+      <c r="F24" s="13">
+        <f t="shared" si="3"/>
+        <v>-34.4815</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="13">
+        <f t="shared" si="1"/>
+        <v>5.7074</v>
+      </c>
+      <c r="E25" s="13">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F25" s="13">
+        <f t="shared" si="3"/>
+        <v>-36.08</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="13">
+        <f t="shared" si="1"/>
+        <v>6.0122</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="F26" s="13">
+        <f t="shared" si="3"/>
+        <v>-37.6215</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="13">
+        <f t="shared" si="1"/>
+        <v>6.317</v>
+      </c>
+      <c r="E27" s="13">
+        <f t="shared" si="4"/>
+        <v>2.2</v>
+      </c>
+      <c r="F27" s="13">
+        <f t="shared" si="3"/>
+        <v>-39.106</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" s="13">
+        <f t="shared" si="4"/>
+        <v>2.54</v>
+      </c>
+      <c r="F28" s="13">
+        <f t="shared" si="3"/>
+        <v>-43.72694</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" s="13">
+        <f t="shared" si="4"/>
+        <v>3.2</v>
+      </c>
+      <c r="F29" s="13">
+        <f t="shared" si="3"/>
+        <v>-50.816</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -12500,277 +12758,277 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26">
@@ -12778,10 +13036,10 @@
         <v>30</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -12804,183 +13062,183 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B2" s="18"/>
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B3" s="18"/>
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B4" s="18"/>
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B5" s="18"/>
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B6" s="18"/>
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B7" s="18"/>
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B8" s="18"/>
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B9" s="18"/>
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B10" s="18"/>
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B11" s="18"/>
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B12" s="18"/>
     </row>
     <row r="13">
       <c r="A13" s="19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B13" s="18"/>
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B14" s="18"/>
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B15" s="18"/>
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B16" s="18"/>
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B17" s="18"/>
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B18" s="18"/>
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B19" s="18"/>
     </row>
     <row r="20">
       <c r="A20" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B20" s="18"/>
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B21" s="18"/>
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B22" s="18"/>
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B23" s="18"/>
     </row>
     <row r="24">
       <c r="A24" s="20" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B24" s="18"/>
     </row>
     <row r="25">
       <c r="A25" s="20" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B25" s="18"/>
     </row>
     <row r="26">
       <c r="A26" s="19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B26" s="18"/>
     </row>
     <row r="27">
       <c r="A27" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B27" s="18"/>
     </row>
     <row r="28">
       <c r="A28" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B28" s="18"/>
     </row>
     <row r="29">
       <c r="A29" s="21" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B29" s="18"/>
     </row>
     <row r="30">
       <c r="A30" s="22" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B30" s="18"/>
     </row>

</xml_diff>

<commit_message>
Updated State Diagram, Excel Sheet, and Added state transtions
</commit_message>
<xml_diff>
--- a/CodeDocumentation/2024 Cresendo.xlsx
+++ b/CodeDocumentation/2024 Cresendo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MZS5XJ\Documents\FRC\2024Crescendo\CodeDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F4C702-C8F2-46AB-AA8C-9E0C62C99BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D74E29-330B-403A-9A75-4B48041148E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="345" windowWidth="22545" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pratice Bot Config" sheetId="1" r:id="rId1"/>
@@ -772,15 +772,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -804,6 +795,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1358,20 +1358,20 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:12" ht="12.75">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="22"/>
-      <c r="I3" s="20" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
+      <c r="I3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="22"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="31"/>
     </row>
     <row r="4" spans="2:12" ht="12.75">
       <c r="B4" s="2" t="s">
@@ -1746,19 +1746,19 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:11" ht="12.75">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="I20" s="20" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="31"/>
+      <c r="I20" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="22"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="31"/>
     </row>
     <row r="21" spans="2:11" ht="12.75">
       <c r="B21" s="2" t="s">
@@ -2005,19 +2005,19 @@
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="2:11" ht="12.75">
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="I33" s="20" t="s">
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="31"/>
+      <c r="I33" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="J33" s="21"/>
-      <c r="K33" s="22"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="31"/>
     </row>
     <row r="34" spans="2:11" ht="12.75">
       <c r="B34" s="2" t="s">
@@ -6932,7 +6932,7 @@
   <dimension ref="B1:L995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -6947,7 +6947,7 @@
     <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6962,20 +6962,20 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="22"/>
-      <c r="I3" s="20" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
+      <c r="I3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="22"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="31"/>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="2" t="s">
@@ -7188,16 +7188,16 @@
       <c r="G10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="25" t="s">
+      <c r="K10" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="26">
+      <c r="L10" s="21">
         <v>6</v>
       </c>
     </row>
@@ -7220,16 +7220,16 @@
       <c r="G11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="27" t="s">
+      <c r="K11" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="28">
+      <c r="L11" s="23">
         <v>7</v>
       </c>
     </row>
@@ -7252,16 +7252,16 @@
       <c r="G12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="29" t="s">
+      <c r="J12" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="K12" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="L12" s="30"/>
+      <c r="L12" s="25"/>
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="4" t="s">
@@ -7282,16 +7282,16 @@
       <c r="G13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="29" t="s">
+      <c r="J13" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="27" t="s">
+      <c r="K13" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="30"/>
+      <c r="L13" s="25"/>
     </row>
     <row r="14" spans="2:12">
       <c r="B14" s="1"/>
@@ -7300,16 +7300,16 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="I14" s="27" t="s">
+      <c r="I14" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="K14" s="27" t="s">
+      <c r="K14" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="L14" s="30"/>
+      <c r="L14" s="25"/>
     </row>
     <row r="15" spans="2:12">
       <c r="B15" s="1"/>
@@ -7318,31 +7318,31 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="27" t="s">
+      <c r="K15" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="30"/>
+      <c r="L15" s="25"/>
     </row>
     <row r="16" spans="2:12">
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="I16" s="29" t="s">
+      <c r="I16" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="J16" s="31" t="s">
+      <c r="J16" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="K16" s="32" t="s">
+      <c r="K16" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="L16" s="33"/>
+      <c r="L16" s="28"/>
     </row>
     <row r="17" spans="2:11">
       <c r="E17" s="1"/>
@@ -7360,19 +7360,19 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="I20" s="20" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="31"/>
+      <c r="I20" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="22"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="31"/>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
@@ -7615,19 +7615,19 @@
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="2:11">
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="I33" s="20" t="s">
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="31"/>
+      <c r="I33" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="J33" s="21"/>
-      <c r="K33" s="22"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="31"/>
     </row>
     <row r="34" spans="2:11">
       <c r="B34" s="2" t="s">
@@ -12549,14 +12549,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="D1" s="23" t="s">
+      <c r="B1" s="33"/>
+      <c r="D1" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="24"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="8" t="s">
@@ -12958,175 +12958,175 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="14" t="s">
         <v>135</v>
       </c>
       <c r="B2" s="15"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="14" t="s">
         <v>91</v>
       </c>
       <c r="B3" s="15"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="14" t="s">
         <v>136</v>
       </c>
       <c r="B4" s="15"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="14.25">
       <c r="A5" s="14" t="s">
         <v>137</v>
       </c>
       <c r="B5" s="15"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="14.25">
       <c r="A6" s="14" t="s">
         <v>138</v>
       </c>
       <c r="B6" s="15"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" ht="14.25">
       <c r="A7" s="14" t="s">
         <v>139</v>
       </c>
       <c r="B7" s="15"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="14.25">
       <c r="A8" s="14" t="s">
         <v>140</v>
       </c>
       <c r="B8" s="15"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="14.25">
       <c r="A9" s="14" t="s">
         <v>141</v>
       </c>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="14.25">
       <c r="A10" s="14" t="s">
         <v>142</v>
       </c>
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="14.25">
       <c r="A11" s="14" t="s">
         <v>143</v>
       </c>
       <c r="B11" s="15"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="14.25">
       <c r="A12" s="14" t="s">
         <v>144</v>
       </c>
       <c r="B12" s="15"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="14.25">
       <c r="A13" s="16" t="s">
         <v>145</v>
       </c>
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="14.25">
       <c r="A14" s="14" t="s">
         <v>146</v>
       </c>
       <c r="B14" s="15"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="14.25">
       <c r="A15" s="14" t="s">
         <v>147</v>
       </c>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="14.25">
       <c r="A16" s="14" t="s">
         <v>148</v>
       </c>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="14.25">
       <c r="A17" s="14" t="s">
         <v>149</v>
       </c>
       <c r="B17" s="15"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="14.25">
       <c r="A18" s="14" t="s">
         <v>150</v>
       </c>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="14.25">
       <c r="A19" s="14" t="s">
         <v>151</v>
       </c>
       <c r="B19" s="15"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="14.25">
       <c r="A20" s="14" t="s">
         <v>152</v>
       </c>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="14.25">
       <c r="A21" s="14" t="s">
         <v>153</v>
       </c>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="14.25">
       <c r="A22" s="14" t="s">
         <v>154</v>
       </c>
       <c r="B22" s="15"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" ht="14.25">
       <c r="A23" s="14" t="s">
         <v>155</v>
       </c>
       <c r="B23" s="15"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="14.25">
       <c r="A24" s="17" t="s">
         <v>156</v>
       </c>
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" ht="14.25">
       <c r="A25" s="17" t="s">
         <v>157</v>
       </c>
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" ht="14.25">
       <c r="A26" s="16" t="s">
         <v>158</v>
       </c>
       <c r="B26" s="15"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" ht="14.25">
       <c r="A27" s="14" t="s">
         <v>159</v>
       </c>
       <c r="B27" s="15"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" ht="14.25">
       <c r="A28" s="14" t="s">
         <v>160</v>
       </c>
       <c r="B28" s="15"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" ht="14.25">
       <c r="A29" s="18" t="s">
         <v>161</v>
       </c>
       <c r="B29" s="15"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" ht="14.25">
       <c r="A30" s="19" t="s">
         <v>162</v>
       </c>

</xml_diff>